<commit_message>
Register send Verify email and Register User from Excel file
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB955099-02E4-4E34-84F4-90CA9E87886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA6AFEE-5498-4919-9769-08D99C44D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,76 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Field1</t>
-  </si>
-  <si>
-    <t>Field2</t>
-  </si>
-  <si>
-    <t>Field3</t>
-  </si>
-  <si>
-    <t>data22</t>
-  </si>
-  <si>
-    <t>data21</t>
-  </si>
-  <si>
-    <t>data23</t>
-  </si>
-  <si>
-    <t>data31</t>
-  </si>
-  <si>
-    <t>data32</t>
-  </si>
-  <si>
-    <t>data33</t>
-  </si>
-  <si>
-    <t>data41</t>
-  </si>
-  <si>
-    <t>data42</t>
-  </si>
-  <si>
-    <t>data43</t>
-  </si>
-  <si>
-    <t>data51</t>
-  </si>
-  <si>
-    <t>data52</t>
-  </si>
-  <si>
-    <t>data53</t>
-  </si>
-  <si>
-    <t>data61</t>
-  </si>
-  <si>
-    <t>data62</t>
-  </si>
-  <si>
-    <t>data63</t>
-  </si>
-  <si>
-    <t>data00</t>
-  </si>
-  <si>
-    <t>data01</t>
-  </si>
-  <si>
-    <t>data02</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>bocaioandoru12@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>birlea24@gmail.com</t>
+  </si>
+  <si>
+    <t>Alex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +65,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,13 +95,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,13 +417,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419E23F4-DD5D-4C26-ADA2-A2F3675EFC65}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -465,73 +441,32 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F4EAC490-DB10-4F23-83E3-557F21B471E6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Register send Verify email and Register User from Excel file (#14)
Co-authored-by: Doru <doru.boca@cityscroller.com>
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB955099-02E4-4E34-84F4-90CA9E87886A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA6AFEE-5498-4919-9769-08D99C44D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,76 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Field1</t>
-  </si>
-  <si>
-    <t>Field2</t>
-  </si>
-  <si>
-    <t>Field3</t>
-  </si>
-  <si>
-    <t>data22</t>
-  </si>
-  <si>
-    <t>data21</t>
-  </si>
-  <si>
-    <t>data23</t>
-  </si>
-  <si>
-    <t>data31</t>
-  </si>
-  <si>
-    <t>data32</t>
-  </si>
-  <si>
-    <t>data33</t>
-  </si>
-  <si>
-    <t>data41</t>
-  </si>
-  <si>
-    <t>data42</t>
-  </si>
-  <si>
-    <t>data43</t>
-  </si>
-  <si>
-    <t>data51</t>
-  </si>
-  <si>
-    <t>data52</t>
-  </si>
-  <si>
-    <t>data53</t>
-  </si>
-  <si>
-    <t>data61</t>
-  </si>
-  <si>
-    <t>data62</t>
-  </si>
-  <si>
-    <t>data63</t>
-  </si>
-  <si>
-    <t>data00</t>
-  </si>
-  <si>
-    <t>data01</t>
-  </si>
-  <si>
-    <t>data02</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>bocaioandoru12@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>birlea24@gmail.com</t>
+  </si>
+  <si>
+    <t>Alex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +65,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,13 +95,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,13 +417,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419E23F4-DD5D-4C26-ADA2-A2F3675EFC65}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -465,73 +441,32 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F4EAC490-DB10-4F23-83E3-557F21B471E6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
JWT Bearer with Auth Role base Scheme, CampusEndpoint wrapper & Small Service fixes
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\facultate\AN 3 S1\IS\campus-server\FileStorage\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA6AFEE-5498-4919-9769-08D99C44D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AAAA1A-63E8-4697-9E94-0B8EA6AB153F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Alex</t>
+  </si>
+  <si>
+    <t>Professor</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
JWT Bearer, Auth Scheme, Endpoints Wrapper (#16)
Co-authored-by: Doru <doru.boca@cityscroller.com>
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\facultate\AN 3 S1\IS\campus-server\FileStorage\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA6AFEE-5498-4919-9769-08D99C44D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AAAA1A-63E8-4697-9E94-0B8EA6AB153F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Alex</t>
+  </si>
+  <si>
+    <t>Professor</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
MongoDB implemntation, Excel database storage & HTTP Endpoint error fix (#18)
Co-authored-by: Doru <doru.boca@cityscroller.com>
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\facultate\AN 3 S1\IS\campus-server\FileStorage\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AAAA1A-63E8-4697-9E94-0B8EA6AB153F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4212F0-1598-4816-ACF9-A3B3DE6F86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Email</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>Professor</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+1@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru2</t>
+  </si>
+  <si>
+    <t>Management</t>
   </si>
 </sst>
 </file>
@@ -420,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419E23F4-DD5D-4C26-ADA2-A2F3675EFC65}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,10 +474,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F4EAC490-DB10-4F23-83E3-557F21B471E6}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{621359A1-90A6-4F91-A845-AAC9FBEAD5B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bulk register logic finished
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE8FF4-5C02-4727-BCCD-587342E7934F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008C9180-CEDF-42CA-BC55-E779A3089CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
+    <workbookView xWindow="28680" yWindow="-6990" windowWidth="29040" windowHeight="16440" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Email</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Role</t>
   </si>
   <si>
-    <t>bocaioandoru12@gmail.com</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Doru0</t>
-  </si>
-  <si>
     <t>AC</t>
   </si>
   <si>
@@ -108,16 +102,16 @@
     <t>Major</t>
   </si>
   <si>
-    <t>Campus</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
     <t>CTI</t>
   </si>
   <si>
     <t>AIA</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+5@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru5</t>
   </si>
 </sst>
 </file>
@@ -486,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419E23F4-DD5D-4C26-ADA2-A2F3675EFC65}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,9 +493,10 @@
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
     <col min="5" max="5" width="12.21875" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,73 +507,67 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -587,21 +576,21 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -610,27 +599,21 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>106</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bulk User operations (#28)
Co-authored-by: Doru <doru.boca@cityscroller.com>
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4212F0-1598-4816-ACF9-A3B3DE6F86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3595D23-7D83-454E-A30B-97497D11B2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Email</t>
   </si>
@@ -36,21 +36,9 @@
     <t>Role</t>
   </si>
   <si>
-    <t>bocaioandoru12@gmail.com</t>
-  </si>
-  <si>
-    <t>Doru</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
-    <t>birlea24@gmail.com</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>Professor</t>
   </si>
   <si>
@@ -61,6 +49,69 @@
   </si>
   <si>
     <t>Management</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+2@gmail.com</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+3@gmail.com</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+4@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru3</t>
+  </si>
+  <si>
+    <t>Doru1</t>
+  </si>
+  <si>
+    <t>Doru4</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>UTCN</t>
+  </si>
+  <si>
+    <t>Campus_Student</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Prof. Eng.</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>CTI</t>
+  </si>
+  <si>
+    <t>AIA</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+5@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru5</t>
   </si>
 </sst>
 </file>
@@ -429,19 +480,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419E23F4-DD5D-4C26-ADA2-A2F3675EFC65}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,45 +506,124 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F4EAC490-DB10-4F23-83E3-557F21B471E6}"/>
-    <hyperlink ref="A4" r:id="rId2" xr:uid="{621359A1-90A6-4F91-A845-AAC9FBEAD5B7}"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{247CD742-F63E-496A-9A2B-3B820ED5B8C0}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{B8C65CF6-5FB1-4157-8BBE-11BB7F120967}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{21EB0403-0B58-48EB-A7E8-6B440A836D9A}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{7A72A0DB-7424-4765-AEB1-2C086067E8A6}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{53019179-F0F0-4FE4-B406-7AB95BDCE124}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial Implementationg & RPC endpoints for Grades Service
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3595D23-7D83-454E-A30B-97497D11B2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7142D6-E008-436D-A068-8FD670DE088B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Email</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Student</t>
   </si>
   <si>
-    <t>Professor</t>
-  </si>
-  <si>
     <t>bocaioandoru12+1@gmail.com</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>UTCN</t>
   </si>
   <si>
-    <t>Campus_Student</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -85,12 +79,6 @@
   </si>
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Prof. Eng.</t>
   </si>
   <si>
     <t>Year</t>
@@ -483,7 +471,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,67 +495,70 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -576,21 +567,21 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -599,18 +590,18 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
unfinished campus service (#29)
Co-authored-by: Doru <doru.boca@cityscroller.com>
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7142D6-E008-436D-A068-8FD670DE088B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BBDF8D-422B-4FB7-9A66-021929F7552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Email</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Doru5</t>
+  </si>
+  <si>
+    <t>Professor</t>
+  </si>
+  <si>
+    <t>Eng.</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Campus_Student</t>
   </si>
 </sst>
 </file>
@@ -471,7 +483,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,7 +544,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -545,6 +557,12 @@
       </c>
       <c r="G3" t="s">
         <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -578,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Secrets added using .env
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BBDF8D-422B-4FB7-9A66-021929F7552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C987C96-96DA-4139-A428-5907034C097F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
+    <workbookView xWindow="28680" yWindow="-6990" windowWidth="29040" windowHeight="16440" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Email</t>
   </si>
@@ -39,79 +39,55 @@
     <t>Student</t>
   </si>
   <si>
-    <t>bocaioandoru12+1@gmail.com</t>
+    <t>bocaioandoru12+3@gmail.com</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+4@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru3</t>
+  </si>
+  <si>
+    <t>Doru4</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>UTCN</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>CTI</t>
+  </si>
+  <si>
+    <t>Campus_Student</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+2@gmail.com</t>
   </si>
   <si>
     <t>Doru2</t>
   </si>
   <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+2@gmail.com</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+3@gmail.com</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+4@gmail.com</t>
-  </si>
-  <si>
-    <t>Doru3</t>
-  </si>
-  <si>
-    <t>Doru1</t>
-  </si>
-  <si>
-    <t>Doru4</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>UTCN</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>CTI</t>
-  </si>
-  <si>
-    <t>AIA</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+5@gmail.com</t>
-  </si>
-  <si>
-    <t>Doru5</t>
-  </si>
-  <si>
     <t>Professor</t>
   </si>
   <si>
     <t>Eng.</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Campus_Student</t>
   </si>
 </sst>
 </file>
@@ -483,7 +459,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,22 +483,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -530,97 +506,69 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -628,11 +576,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{247CD742-F63E-496A-9A2B-3B820ED5B8C0}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{B8C65CF6-5FB1-4157-8BBE-11BB7F120967}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{21EB0403-0B58-48EB-A7E8-6B440A836D9A}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{7A72A0DB-7424-4765-AEB1-2C086067E8A6}"/>
-    <hyperlink ref="A2" r:id="rId5" xr:uid="{53019179-F0F0-4FE4-B406-7AB95BDCE124}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{247CD742-F63E-496A-9A2B-3B820ED5B8C0}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{B8C65CF6-5FB1-4157-8BBE-11BB7F120967}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Secrets added using .env (#37)
Co-authored-by: Doru <doru.boca@cityscroller.com>
</commit_message>
<xml_diff>
--- a/FileStorage/ExcelFiles/Book1.xlsx
+++ b/FileStorage/ExcelFiles/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bocai\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BBDF8D-422B-4FB7-9A66-021929F7552D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C987C96-96DA-4139-A428-5907034C097F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
+    <workbookView xWindow="28680" yWindow="-6990" windowWidth="29040" windowHeight="16440" xr2:uid="{D36BC047-7F5E-4CAC-B9BB-58A8D911F535}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Email</t>
   </si>
@@ -39,79 +39,55 @@
     <t>Student</t>
   </si>
   <si>
-    <t>bocaioandoru12+1@gmail.com</t>
+    <t>bocaioandoru12+3@gmail.com</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+4@gmail.com</t>
+  </si>
+  <si>
+    <t>Doru3</t>
+  </si>
+  <si>
+    <t>Doru4</t>
+  </si>
+  <si>
+    <t>University</t>
+  </si>
+  <si>
+    <t>UTCN</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>CTI</t>
+  </si>
+  <si>
+    <t>Campus_Student</t>
+  </si>
+  <si>
+    <t>bocaioandoru12+2@gmail.com</t>
   </si>
   <si>
     <t>Doru2</t>
   </si>
   <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+2@gmail.com</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+3@gmail.com</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+4@gmail.com</t>
-  </si>
-  <si>
-    <t>Doru3</t>
-  </si>
-  <si>
-    <t>Doru1</t>
-  </si>
-  <si>
-    <t>Doru4</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>UTCN</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>CTI</t>
-  </si>
-  <si>
-    <t>AIA</t>
-  </si>
-  <si>
-    <t>bocaioandoru12+5@gmail.com</t>
-  </si>
-  <si>
-    <t>Doru5</t>
-  </si>
-  <si>
     <t>Professor</t>
   </si>
   <si>
     <t>Eng.</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>Campus_Student</t>
   </si>
 </sst>
 </file>
@@ -483,7 +459,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -507,22 +483,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -530,97 +506,69 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -628,11 +576,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{247CD742-F63E-496A-9A2B-3B820ED5B8C0}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{B8C65CF6-5FB1-4157-8BBE-11BB7F120967}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{21EB0403-0B58-48EB-A7E8-6B440A836D9A}"/>
-    <hyperlink ref="A3" r:id="rId4" xr:uid="{7A72A0DB-7424-4765-AEB1-2C086067E8A6}"/>
-    <hyperlink ref="A2" r:id="rId5" xr:uid="{53019179-F0F0-4FE4-B406-7AB95BDCE124}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{247CD742-F63E-496A-9A2B-3B820ED5B8C0}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{B8C65CF6-5FB1-4157-8BBE-11BB7F120967}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>